<commit_message>
Examined absolute layoffs by IPO status
</commit_message>
<xml_diff>
--- a/tech_layoffs_analysis/results/tech_layoffs_results.xlsx
+++ b/tech_layoffs_analysis/results/tech_layoffs_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbryant/Documents/GitHub/SQL_Projects/tech_layoffs_research/exports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbryant/Documents/GitHub/SQL_Projects/tech_layoffs_analysis/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B4D75F-EFF6-9846-841E-73D7CEBEA968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3BD549-7ABA-194D-911C-7B0BE37A0808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{D5FE2044-42E5-F445-8EAD-A3BDB9DA7242}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Seattle</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>LAYOFFS BY IPO STATUS</t>
+  </si>
+  <si>
+    <t>num_layoffs</t>
   </si>
 </sst>
 </file>
@@ -4586,41 +4589,50 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DEAB901-DE36-DF40-8BD5-2B8A2ADA5737}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3">
         <v>172</v>
       </c>
+      <c r="C3">
+        <v>24758</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4">
         <v>68</v>
+      </c>
+      <c r="C4">
+        <v>60051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>